<commit_message>
Few corrections for ExcelReader
</commit_message>
<xml_diff>
--- a/vechicleenquiry/src/main/resources/TestVehicle/test-vehicle.xlsx
+++ b/vechicleenquiry/src/main/resources/TestVehicle/test-vehicle.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28308"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karthi-Job\dvla-tests\vechicleenquiry\src\main\resources\TestVehicle\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{20CFEFF4-0153-440A-81FA-98D3FDD10057}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,19 +27,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Nissan</t>
+    <t>YM15 ZYU</t>
   </si>
   <si>
-    <t>white</t>
+    <t>JAGUAR</t>
   </si>
   <si>
-    <t>DG10 HGE</t>
+    <t>red</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -77,6 +83,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,22 +415,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>